<commit_message>
chore: updated equitherm calculator
</commit_message>
<xml_diff>
--- a/assets/equitherm_calc.xlsx
+++ b/assets/equitherm_calc.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Projects\otgateway\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\otgateway\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2ADFF3B-2C07-4BCB-9117-ADC34678897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19187" windowHeight="6960"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="12835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Outdoor temp</t>
   </si>
@@ -161,15 +171,18 @@
       <t xml:space="preserve"> - raw heating temperature (N result)</t>
     </r>
   </si>
+  <si>
+    <t>N + K + T limited</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="#0.0&quot; °&quot;"/>
+    <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +225,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -396,12 +417,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
@@ -418,7 +439,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -431,15 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -467,18 +480,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="176" formatCode="#0.0&quot; °&quot;"/>
+      <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode="#0.0&quot; °&quot;"/>
+      <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#0.0&quot; °&quot;"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color theme="1"/>
+        </left>
+        <right style="thick">
+          <color theme="1"/>
+        </right>
+        <top style="thick">
+          <color theme="1"/>
+        </top>
+        <bottom style="thick">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <protection locked="1" hidden="0"/>
@@ -518,39 +576,13 @@
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="#0.0&quot; °&quot;"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode="#0.0&quot; °&quot;"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color theme="1"/>
-        </left>
-        <right style="thick">
-          <color theme="1"/>
-        </right>
-        <top style="thick">
-          <color theme="1"/>
-        </top>
-        <bottom style="thick">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thick">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -578,46 +610,54 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9707295270303521E-2"/>
+          <c:y val="1.2140032503368509E-2"/>
+          <c:w val="0.92452028031062872"/>
+          <c:h val="0.84560395247644138"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$1</c:f>
+              <c:f>Лист1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N + K + T result</c:v>
+                  <c:v>N result</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:miter lim="800000"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="diamond"/>
             <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -789,162 +829,162 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$52</c:f>
+              <c:f>Лист1!$B$2:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>#0.0" °"</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
+                  <c:v>20.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>34.700000000000003</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>37.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>38.700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="12">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>41.3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>42.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43.9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="18">
+                  <c:v>42.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>46.3</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>47.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>48.7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>49.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>52.1</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="23">
+                  <c:v>47.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>48.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>49.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>51.6</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>52.4</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>53.2</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>54.3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>55.3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>56.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>57.4</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>58.4</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>59.3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>60.3</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="31">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>54.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>55.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>56.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>56.9</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>57.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>58.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>58.9</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>59.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>60.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>60.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>61.2</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>62.1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>63</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>63.9</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>64.8</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>65.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>66.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>67.2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>68.7</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>69.5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>70.2</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>70.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>71.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>72.2</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>72.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>73.5</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>74.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>74.7</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>75.2</c:v>
-                </c:pt>
                 <c:pt idx="43">
-                  <c:v>75.8</c:v>
+                  <c:v>61.8</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>76.3</c:v>
+                  <c:v>62.3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>76.8</c:v>
+                  <c:v>62.8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>77.2</c:v>
+                  <c:v>63.2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>77.7</c:v>
+                  <c:v>63.7</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>78.099999999999994</c:v>
+                  <c:v>64.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>78.599999999999994</c:v>
+                  <c:v>64.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>79</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,7 +992,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000002C-6335-4E08-8A78-0CD47DD49ABC}"/>
+              <c16:uniqueId val="{0000002D-6335-4E08-8A78-0CD47DD49ABC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -971,27 +1011,25 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:miter lim="800000"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1331,42 +1369,39 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$B$1</c:f>
+              <c:f>Лист1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>N result</c:v>
+                  <c:v>N + K + T result</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg2">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:miter lim="800000"/>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="diamond"/>
             <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="bg1"/>
+                  <a:schemeClr val="accent4"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -1538,162 +1573,162 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$52</c:f>
+              <c:f>Лист1!$D$2:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>#0.0" °"</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>20.7</c:v>
+                  <c:v>34.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.4</c:v>
+                  <c:v>37.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.7</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27.3</c:v>
+                  <c:v>41.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.6</c:v>
+                  <c:v>42.6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29.9</c:v>
+                  <c:v>43.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>31.1</c:v>
+                  <c:v>45.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>46.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>33.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.700000000000003</c:v>
+                  <c:v>48.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>35.799999999999997</c:v>
+                  <c:v>49.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>38.1</c:v>
+                  <c:v>52.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39.200000000000003</c:v>
+                  <c:v>53.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>40.299999999999997</c:v>
+                  <c:v>54.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41.3</c:v>
+                  <c:v>55.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42.4</c:v>
+                  <c:v>56.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43.4</c:v>
+                  <c:v>57.4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>44.4</c:v>
+                  <c:v>58.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>45.3</c:v>
+                  <c:v>59.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>46.3</c:v>
+                  <c:v>60.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>47.2</c:v>
+                  <c:v>61.2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>48.1</c:v>
+                  <c:v>62.1</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>49.9</c:v>
+                  <c:v>63.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>50.8</c:v>
+                  <c:v>64.8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>51.6</c:v>
+                  <c:v>65.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>52.4</c:v>
+                  <c:v>66.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>53.2</c:v>
+                  <c:v>67.2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>54</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>54.7</c:v>
+                  <c:v>68.7</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>55.5</c:v>
+                  <c:v>69.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56.2</c:v>
+                  <c:v>70.2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>56.9</c:v>
+                  <c:v>70.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>57.6</c:v>
+                  <c:v>71.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>58.2</c:v>
+                  <c:v>72.2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>58.9</c:v>
+                  <c:v>72.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>59.5</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>60.1</c:v>
+                  <c:v>74.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>60.7</c:v>
+                  <c:v>74.7</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>61.2</c:v>
+                  <c:v>75.2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>61.8</c:v>
+                  <c:v>75.8</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>62.3</c:v>
+                  <c:v>76.3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>62.8</c:v>
+                  <c:v>76.8</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>63.2</c:v>
+                  <c:v>77.2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>63.7</c:v>
+                  <c:v>77.7</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>64.099999999999994</c:v>
+                  <c:v>78.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>64.599999999999994</c:v>
+                  <c:v>78.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>65</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1701,7 +1736,379 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000002D-6335-4E08-8A78-0CD47DD49ABC}"/>
+              <c16:uniqueId val="{0000002C-6335-4E08-8A78-0CD47DD49ABC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N + K + T limited</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$A$2:$A$52</c:f>
+              <c:numCache>
+                <c:formatCode>#0.0" °"</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-18</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-19</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-22</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-26</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-27</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-29</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$E$2:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>#0.0" °"</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>52.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>53.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>54.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>55.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>57.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>58.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59.3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>60.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>61.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62.1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>63.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64.8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>65.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>66.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>67.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>68.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>70.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>71.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>72.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>74.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>75.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>75.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>76.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>76.8</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>77.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>77.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>78.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>78.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6DF8-493F-AC59-08DAD03CCCBE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1733,7 +2140,6 @@
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
-                  <a:alpha val="32000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1742,12 +2148,12 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="#0.0&quot; °&quot;" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
@@ -1755,12 +2161,11 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
-            <a:tailEnd type="none" w="med" len="lg"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1800,7 +2205,6 @@
                 <a:schemeClr val="tx1">
                   <a:lumMod val="15000"/>
                   <a:lumOff val="85000"/>
-                  <a:alpha val="32000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1809,25 +2213,23 @@
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="#0.0&quot; °&quot;" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln>
             <a:solidFill>
               <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
-            <a:round/>
-            <a:tailEnd type="none" w="med" len="lg"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1849,6 +2251,7 @@
         <c:crossAx val="1494704223"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1858,6 +2261,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="0"/>
@@ -1936,7 +2370,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="237">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1947,7 +2381,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1960,7 +2394,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -1968,7 +2402,6 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
-        <a:tailEnd type="none" w="med" len="lg"/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1994,7 +2427,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2038,7 +2471,47 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
@@ -2046,73 +2519,19 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="38100" cap="flat" cmpd="dbl" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2137,13 +2556,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2153,13 +2574,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
@@ -2180,13 +2601,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2198,13 +2620,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2215,6 +2638,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2229,7 +2658,6 @@
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
-            <a:alpha val="32000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2244,14 +2672,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
-            <a:alpha val="32000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2263,10 +2691,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2278,13 +2710,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2321,20 +2754,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-        <a:tailEnd type="none" w="med" len="lg"/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2345,13 +2769,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -2361,11 +2786,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2377,7 +2802,12 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="rnd"/>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
     </cs:spPr>
   </cs:trendline>
   <cs:trendlineLabel>
@@ -2397,7 +2827,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2406,8 +2836,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2423,18 +2853,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-        <a:tailEnd type="none" w="med" len="lg"/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2444,6 +2862,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2452,20 +2876,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>543981</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3298</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>15903</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>174928</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2484,18 +2914,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Таблица4" displayName="Таблица4" ref="A1:D52" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:D52"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Outdoor temp" dataDxfId="5"/>
-    <tableColumn id="2" name="N result" dataDxfId="4">
-      <calculatedColumnFormula>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A2 + 5) * (-0.2 * A2 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A2 + 5)) + (-5.06 * F$2 + 18.06), 1)))</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица4" displayName="Таблица4" ref="A1:E52" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6">
+  <autoFilter ref="A1:E52" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Outdoor temp" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="N result" dataDxfId="3">
+      <calculatedColumnFormula>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A2 + 5) * (-0.2 * A2 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A2 + 5)) + (-5.06 * G$2 + 18.06), 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="N + K result" dataDxfId="1">
-      <calculatedColumnFormula>MIN(K$2, MAX(L$2, B2+N$2))</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="N + K result" dataDxfId="2">
+      <calculatedColumnFormula>B2+O$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="N + K + T result" dataDxfId="0">
-      <calculatedColumnFormula>MIN(K$2, MAX(L$2, C2+O$2))</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="N + K + T result" dataDxfId="1">
+      <calculatedColumnFormula>C2+P$2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{BB6783CC-A8B3-4B0E-B22A-463D47E8C8DA}" name="N + K + T limited" dataDxfId="0">
+      <calculatedColumnFormula>MIN(L$2, MAX(M$2, D2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2764,29 +3197,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.8203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.76171875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" style="5" customWidth="1"/>
     <col min="3" max="3" width="17" style="5" customWidth="1"/>
-    <col min="4" max="4" width="17.87890625" style="3" customWidth="1"/>
-    <col min="5" max="8" width="7.64453125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.64453125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="12.3515625" style="5" customWidth="1"/>
-    <col min="11" max="12" width="10.64453125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="20.64453125" style="5" customWidth="1"/>
-    <col min="14" max="16384" width="8.9375" style="5"/>
+    <col min="4" max="4" width="17.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="5" customWidth="1"/>
+    <col min="6" max="8" width="7.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" ht="16.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2799,1001 +3234,1237 @@
       <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="16.3" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
         <v>20</v>
       </c>
       <c r="B2" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A2 + 5) * (-0.2 * A2 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A2 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A2 + 5) * (-0.2 * A2 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A2 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>20.7</v>
       </c>
       <c r="C2" s="11">
-        <f>MIN(K$2, MAX(L$2, B2+N$2))</f>
+        <f>B2+O$2</f>
         <v>30.7</v>
       </c>
       <c r="D2" s="11">
-        <f>MIN(K$2, MAX(L$2, C2+O$2))</f>
+        <f t="shared" ref="D2:D33" si="0">C2+P$2</f>
         <v>34.700000000000003</v>
       </c>
-      <c r="F2" s="6">
+      <c r="E2" s="21">
+        <f t="shared" ref="E2:E33" si="1">MIN(L$2, MAX(M$2, D2))</f>
+        <v>40</v>
+      </c>
+      <c r="G2" s="6">
         <v>0.9</v>
       </c>
-      <c r="G2" s="6">
+      <c r="H2" s="6">
         <v>5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="6">
         <v>2</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>22</v>
       </c>
-      <c r="J2" s="7">
+      <c r="K2" s="7">
         <v>19</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>90</v>
       </c>
-      <c r="L2" s="7">
-        <v>20</v>
-      </c>
-      <c r="N2" s="2">
-        <f>(I2 - 20) * G2</f>
+      <c r="M2" s="7">
+        <v>40</v>
+      </c>
+      <c r="O2" s="2">
+        <f>(J2 - 20) * H2</f>
         <v>10</v>
       </c>
-      <c r="O2" s="2">
-        <f>IF((I2-J2) &gt; 2, 2, I2-J2)*H$2</f>
+      <c r="P2" s="2">
+        <f>IF((J2-K2) &gt; 2, 2, J2-K2)*I$2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="14.7" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:16" ht="15.65" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>19</v>
       </c>
       <c r="B3" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A3 + 5) * (-0.2 * A3 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A3 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A3 + 5) * (-0.2 * A3 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A3 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>22</v>
       </c>
       <c r="C3" s="11">
-        <f>MIN(K$2, MAX(L$2, B3+N$2))</f>
+        <f>B3+O$2</f>
         <v>32</v>
       </c>
       <c r="D3" s="11">
-        <f>MIN(K$2, MAX(L$2, C3+O$2))</f>
+        <f t="shared" si="0"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E3" s="21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>18</v>
       </c>
       <c r="B4" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A4 + 5) * (-0.2 * A4 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A4 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A4 + 5) * (-0.2 * A4 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A4 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>23.4</v>
       </c>
       <c r="C4" s="11">
-        <f>MIN(K$2, MAX(L$2, B4+N$2))</f>
+        <f>B4+O$2</f>
         <v>33.4</v>
       </c>
       <c r="D4" s="11">
-        <f>MIN(K$2, MAX(L$2, C4+O$2))</f>
+        <f t="shared" si="0"/>
         <v>37.4</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E4" s="21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>17</v>
       </c>
       <c r="B5" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A5 + 5) * (-0.2 * A5 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A5 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A5 + 5) * (-0.2 * A5 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A5 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>24.7</v>
       </c>
       <c r="C5" s="11">
-        <f>MIN(K$2, MAX(L$2, B5+N$2))</f>
+        <f>B5+O$2</f>
         <v>34.700000000000003</v>
       </c>
       <c r="D5" s="11">
-        <f>MIN(K$2, MAX(L$2, C5+O$2))</f>
+        <f t="shared" si="0"/>
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E5" s="21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>16</v>
       </c>
       <c r="B6" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A6 + 5) * (-0.2 * A6 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A6 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A6 + 5) * (-0.2 * A6 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A6 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>26</v>
       </c>
       <c r="C6" s="11">
-        <f>MIN(K$2, MAX(L$2, B6+N$2))</f>
+        <f>B6+O$2</f>
         <v>36</v>
       </c>
       <c r="D6" s="11">
-        <f>MIN(K$2, MAX(L$2, C6+O$2))</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E6" s="21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>15</v>
       </c>
       <c r="B7" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A7 + 5) * (-0.2 * A7 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A7 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A7 + 5) * (-0.2 * A7 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A7 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>27.3</v>
       </c>
       <c r="C7" s="11">
-        <f>MIN(K$2, MAX(L$2, B7+N$2))</f>
+        <f>B7+O$2</f>
         <v>37.299999999999997</v>
       </c>
       <c r="D7" s="11">
-        <f>MIN(K$2, MAX(L$2, C7+O$2))</f>
+        <f t="shared" si="0"/>
         <v>41.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E7" s="21">
+        <f t="shared" si="1"/>
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>14</v>
       </c>
       <c r="B8" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A8 + 5) * (-0.2 * A8 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A8 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A8 + 5) * (-0.2 * A8 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A8 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>28.6</v>
       </c>
       <c r="C8" s="11">
-        <f>MIN(K$2, MAX(L$2, B8+N$2))</f>
+        <f>B8+O$2</f>
         <v>38.6</v>
       </c>
       <c r="D8" s="11">
-        <f>MIN(K$2, MAX(L$2, C8+O$2))</f>
+        <f t="shared" si="0"/>
         <v>42.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E8" s="21">
+        <f t="shared" si="1"/>
+        <v>42.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>13</v>
       </c>
       <c r="B9" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A9 + 5) * (-0.2 * A9 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A9 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A9 + 5) * (-0.2 * A9 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A9 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>29.9</v>
       </c>
       <c r="C9" s="11">
-        <f>MIN(K$2, MAX(L$2, B9+N$2))</f>
+        <f>B9+O$2</f>
         <v>39.9</v>
       </c>
       <c r="D9" s="11">
-        <f>MIN(K$2, MAX(L$2, C9+O$2))</f>
+        <f t="shared" si="0"/>
         <v>43.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E9" s="21">
+        <f t="shared" si="1"/>
+        <v>43.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>12</v>
       </c>
       <c r="B10" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A10 + 5) * (-0.2 * A10 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A10 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A10 + 5) * (-0.2 * A10 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A10 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>31.1</v>
       </c>
       <c r="C10" s="11">
-        <f>MIN(K$2, MAX(L$2, B10+N$2))</f>
+        <f>B10+O$2</f>
         <v>41.1</v>
       </c>
       <c r="D10" s="11">
-        <f>MIN(K$2, MAX(L$2, C10+O$2))</f>
+        <f t="shared" si="0"/>
         <v>45.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E10" s="21">
+        <f t="shared" si="1"/>
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>11</v>
       </c>
       <c r="B11" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A11 + 5) * (-0.2 * A11 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A11 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A11 + 5) * (-0.2 * A11 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A11 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>32.299999999999997</v>
       </c>
       <c r="C11" s="11">
-        <f>MIN(K$2, MAX(L$2, B11+N$2))</f>
+        <f>B11+O$2</f>
         <v>42.3</v>
       </c>
       <c r="D11" s="11">
-        <f>MIN(K$2, MAX(L$2, C11+O$2))</f>
+        <f t="shared" si="0"/>
         <v>46.3</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E11" s="21">
+        <f t="shared" si="1"/>
+        <v>46.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>10</v>
       </c>
       <c r="B12" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A12 + 5) * (-0.2 * A12 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A12 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A12 + 5) * (-0.2 * A12 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A12 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>33.5</v>
       </c>
       <c r="C12" s="11">
-        <f>MIN(K$2, MAX(L$2, B12+N$2))</f>
+        <f>B12+O$2</f>
         <v>43.5</v>
       </c>
       <c r="D12" s="11">
-        <f>MIN(K$2, MAX(L$2, C12+O$2))</f>
+        <f t="shared" si="0"/>
         <v>47.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E12" s="21">
+        <f t="shared" si="1"/>
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>9</v>
       </c>
       <c r="B13" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A13 + 5) * (-0.2 * A13 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A13 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A13 + 5) * (-0.2 * A13 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A13 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>34.700000000000003</v>
       </c>
       <c r="C13" s="11">
-        <f>MIN(K$2, MAX(L$2, B13+N$2))</f>
+        <f>B13+O$2</f>
         <v>44.7</v>
       </c>
       <c r="D13" s="11">
-        <f>MIN(K$2, MAX(L$2, C13+O$2))</f>
+        <f t="shared" si="0"/>
         <v>48.7</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E13" s="21">
+        <f t="shared" si="1"/>
+        <v>48.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>8</v>
       </c>
       <c r="B14" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A14 + 5) * (-0.2 * A14 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A14 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A14 + 5) * (-0.2 * A14 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A14 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>35.799999999999997</v>
       </c>
       <c r="C14" s="11">
-        <f>MIN(K$2, MAX(L$2, B14+N$2))</f>
+        <f>B14+O$2</f>
         <v>45.8</v>
       </c>
       <c r="D14" s="11">
-        <f>MIN(K$2, MAX(L$2, C14+O$2))</f>
+        <f t="shared" si="0"/>
         <v>49.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E14" s="21">
+        <f t="shared" si="1"/>
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>7</v>
       </c>
       <c r="B15" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A15 + 5) * (-0.2 * A15 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A15 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A15 + 5) * (-0.2 * A15 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A15 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>37</v>
       </c>
       <c r="C15" s="11">
-        <f>MIN(K$2, MAX(L$2, B15+N$2))</f>
+        <f>B15+O$2</f>
         <v>47</v>
       </c>
       <c r="D15" s="11">
-        <f>MIN(K$2, MAX(L$2, C15+O$2))</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E15" s="21">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>6</v>
       </c>
       <c r="B16" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A16 + 5) * (-0.2 * A16 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A16 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A16 + 5) * (-0.2 * A16 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A16 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>38.1</v>
       </c>
       <c r="C16" s="11">
-        <f>MIN(K$2, MAX(L$2, B16+N$2))</f>
+        <f>B16+O$2</f>
         <v>48.1</v>
       </c>
       <c r="D16" s="11">
-        <f>MIN(K$2, MAX(L$2, C16+O$2))</f>
+        <f t="shared" si="0"/>
         <v>52.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E16" s="21">
+        <f t="shared" si="1"/>
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>5</v>
       </c>
       <c r="B17" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A17 + 5) * (-0.2 * A17 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A17 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A17 + 5) * (-0.2 * A17 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A17 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>39.200000000000003</v>
       </c>
       <c r="C17" s="11">
-        <f>MIN(K$2, MAX(L$2, B17+N$2))</f>
+        <f>B17+O$2</f>
         <v>49.2</v>
       </c>
       <c r="D17" s="11">
-        <f>MIN(K$2, MAX(L$2, C17+O$2))</f>
+        <f t="shared" si="0"/>
         <v>53.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E17" s="21">
+        <f t="shared" si="1"/>
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>4</v>
       </c>
       <c r="B18" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A18 + 5) * (-0.2 * A18 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A18 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A18 + 5) * (-0.2 * A18 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A18 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>40.299999999999997</v>
       </c>
       <c r="C18" s="11">
-        <f>MIN(K$2, MAX(L$2, B18+N$2))</f>
+        <f>B18+O$2</f>
         <v>50.3</v>
       </c>
       <c r="D18" s="11">
-        <f>MIN(K$2, MAX(L$2, C18+O$2))</f>
+        <f t="shared" si="0"/>
         <v>54.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E18" s="21">
+        <f t="shared" si="1"/>
+        <v>54.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>3</v>
       </c>
       <c r="B19" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A19 + 5) * (-0.2 * A19 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A19 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A19 + 5) * (-0.2 * A19 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A19 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>41.3</v>
       </c>
       <c r="C19" s="11">
-        <f>MIN(K$2, MAX(L$2, B19+N$2))</f>
+        <f>B19+O$2</f>
         <v>51.3</v>
       </c>
       <c r="D19" s="11">
-        <f>MIN(K$2, MAX(L$2, C19+O$2))</f>
+        <f t="shared" si="0"/>
         <v>55.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E19" s="21">
+        <f t="shared" si="1"/>
+        <v>55.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>2</v>
       </c>
       <c r="B20" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A20 + 5) * (-0.2 * A20 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A20 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A20 + 5) * (-0.2 * A20 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A20 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>42.4</v>
       </c>
       <c r="C20" s="11">
-        <f>MIN(K$2, MAX(L$2, B20+N$2))</f>
+        <f>B20+O$2</f>
         <v>52.4</v>
       </c>
       <c r="D20" s="11">
-        <f>MIN(K$2, MAX(L$2, C20+O$2))</f>
+        <f t="shared" si="0"/>
         <v>56.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E20" s="21">
+        <f t="shared" si="1"/>
+        <v>56.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>1</v>
       </c>
       <c r="B21" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A21 + 5) * (-0.2 * A21 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A21 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A21 + 5) * (-0.2 * A21 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A21 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>43.4</v>
       </c>
       <c r="C21" s="11">
-        <f>MIN(K$2, MAX(L$2, B21+N$2))</f>
+        <f>B21+O$2</f>
         <v>53.4</v>
       </c>
       <c r="D21" s="11">
-        <f>MIN(K$2, MAX(L$2, C21+O$2))</f>
+        <f t="shared" si="0"/>
         <v>57.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E21" s="21">
+        <f t="shared" si="1"/>
+        <v>57.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>0</v>
       </c>
       <c r="B22" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A22 + 5) * (-0.2 * A22 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A22 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A22 + 5) * (-0.2 * A22 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A22 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>44.4</v>
       </c>
       <c r="C22" s="11">
-        <f>MIN(K$2, MAX(L$2, B22+N$2))</f>
+        <f>B22+O$2</f>
         <v>54.4</v>
       </c>
       <c r="D22" s="11">
-        <f>MIN(K$2, MAX(L$2, C22+O$2))</f>
+        <f t="shared" si="0"/>
         <v>58.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E22" s="21">
+        <f t="shared" si="1"/>
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>-1</v>
       </c>
       <c r="B23" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A23 + 5) * (-0.2 * A23 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A23 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A23 + 5) * (-0.2 * A23 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A23 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>45.3</v>
       </c>
       <c r="C23" s="11">
-        <f>MIN(K$2, MAX(L$2, B23+N$2))</f>
+        <f>B23+O$2</f>
         <v>55.3</v>
       </c>
       <c r="D23" s="11">
-        <f>MIN(K$2, MAX(L$2, C23+O$2))</f>
+        <f t="shared" si="0"/>
         <v>59.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E23" s="21">
+        <f t="shared" si="1"/>
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>-2</v>
       </c>
       <c r="B24" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A24 + 5) * (-0.2 * A24 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A24 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A24 + 5) * (-0.2 * A24 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A24 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>46.3</v>
       </c>
       <c r="C24" s="11">
-        <f>MIN(K$2, MAX(L$2, B24+N$2))</f>
+        <f>B24+O$2</f>
         <v>56.3</v>
       </c>
       <c r="D24" s="11">
-        <f>MIN(K$2, MAX(L$2, C24+O$2))</f>
+        <f t="shared" si="0"/>
         <v>60.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E24" s="21">
+        <f t="shared" si="1"/>
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>-3</v>
       </c>
       <c r="B25" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A25 + 5) * (-0.2 * A25 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A25 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A25 + 5) * (-0.2 * A25 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A25 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>47.2</v>
       </c>
       <c r="C25" s="11">
-        <f>MIN(K$2, MAX(L$2, B25+N$2))</f>
+        <f>B25+O$2</f>
         <v>57.2</v>
       </c>
       <c r="D25" s="11">
-        <f>MIN(K$2, MAX(L$2, C25+O$2))</f>
+        <f t="shared" si="0"/>
         <v>61.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E25" s="21">
+        <f t="shared" si="1"/>
+        <v>61.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>-4</v>
       </c>
       <c r="B26" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A26 + 5) * (-0.2 * A26 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A26 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A26 + 5) * (-0.2 * A26 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A26 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>48.1</v>
       </c>
       <c r="C26" s="11">
-        <f>MIN(K$2, MAX(L$2, B26+N$2))</f>
+        <f>B26+O$2</f>
         <v>58.1</v>
       </c>
       <c r="D26" s="11">
-        <f>MIN(K$2, MAX(L$2, C26+O$2))</f>
+        <f t="shared" si="0"/>
         <v>62.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E26" s="21">
+        <f t="shared" si="1"/>
+        <v>62.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>-5</v>
       </c>
       <c r="B27" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A27 + 5) * (-0.2 * A27 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A27 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A27 + 5) * (-0.2 * A27 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A27 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>49</v>
       </c>
       <c r="C27" s="11">
-        <f>MIN(K$2, MAX(L$2, B27+N$2))</f>
+        <f>B27+O$2</f>
         <v>59</v>
       </c>
       <c r="D27" s="11">
-        <f>MIN(K$2, MAX(L$2, C27+O$2))</f>
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E27" s="21">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>-6</v>
       </c>
       <c r="B28" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A28 + 5) * (-0.2 * A28 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A28 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A28 + 5) * (-0.2 * A28 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A28 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>49.9</v>
       </c>
       <c r="C28" s="11">
-        <f>MIN(K$2, MAX(L$2, B28+N$2))</f>
+        <f>B28+O$2</f>
         <v>59.9</v>
       </c>
       <c r="D28" s="11">
-        <f>MIN(K$2, MAX(L$2, C28+O$2))</f>
+        <f t="shared" si="0"/>
         <v>63.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E28" s="21">
+        <f t="shared" si="1"/>
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>-7</v>
       </c>
       <c r="B29" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A29 + 5) * (-0.2 * A29 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A29 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A29 + 5) * (-0.2 * A29 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A29 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>50.8</v>
       </c>
       <c r="C29" s="11">
-        <f>MIN(K$2, MAX(L$2, B29+N$2))</f>
+        <f>B29+O$2</f>
         <v>60.8</v>
       </c>
       <c r="D29" s="11">
-        <f>MIN(K$2, MAX(L$2, C29+O$2))</f>
+        <f t="shared" si="0"/>
         <v>64.8</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="16"/>
-    </row>
-    <row r="30" spans="1:15" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E29" s="21">
+        <f t="shared" si="1"/>
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>-8</v>
       </c>
       <c r="B30" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A30 + 5) * (-0.2 * A30 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A30 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A30 + 5) * (-0.2 * A30 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A30 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>51.6</v>
       </c>
       <c r="C30" s="11">
-        <f>MIN(K$2, MAX(L$2, B30+N$2))</f>
+        <f>B30+O$2</f>
         <v>61.6</v>
       </c>
       <c r="D30" s="11">
-        <f>MIN(K$2, MAX(L$2, C30+O$2))</f>
+        <f t="shared" si="0"/>
         <v>65.599999999999994</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18"/>
-      <c r="O30" s="19"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E30" s="22">
+        <f t="shared" si="1"/>
+        <v>65.599999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>-9</v>
       </c>
       <c r="B31" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A31 + 5) * (-0.2 * A31 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A31 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A31 + 5) * (-0.2 * A31 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A31 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>52.4</v>
       </c>
       <c r="C31" s="11">
-        <f>MIN(K$2, MAX(L$2, B31+N$2))</f>
+        <f>B31+O$2</f>
         <v>62.4</v>
       </c>
       <c r="D31" s="11">
-        <f>MIN(K$2, MAX(L$2, C31+O$2))</f>
+        <f t="shared" si="0"/>
         <v>66.400000000000006</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18"/>
-      <c r="O31" s="19"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E31" s="23">
+        <f t="shared" si="1"/>
+        <v>66.400000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>-10</v>
       </c>
       <c r="B32" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A32 + 5) * (-0.2 * A32 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A32 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A32 + 5) * (-0.2 * A32 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A32 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>53.2</v>
       </c>
       <c r="C32" s="11">
-        <f>MIN(K$2, MAX(L$2, B32+N$2))</f>
+        <f>B32+O$2</f>
         <v>63.2</v>
       </c>
       <c r="D32" s="11">
-        <f>MIN(K$2, MAX(L$2, C32+O$2))</f>
+        <f t="shared" si="0"/>
         <v>67.2</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="19"/>
-    </row>
-    <row r="33" spans="1:15" ht="14.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="E32" s="23">
+        <f t="shared" si="1"/>
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>-11</v>
       </c>
       <c r="B33" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A33 + 5) * (-0.2 * A33 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A33 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A33 + 5) * (-0.2 * A33 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A33 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>54</v>
       </c>
       <c r="C33" s="11">
-        <f>MIN(K$2, MAX(L$2, B33+N$2))</f>
+        <f>B33+O$2</f>
         <v>64</v>
       </c>
       <c r="D33" s="11">
-        <f>MIN(K$2, MAX(L$2, C33+O$2))</f>
+        <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="19"/>
-    </row>
-    <row r="34" spans="1:15" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E33" s="21">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>-12</v>
       </c>
       <c r="B34" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A34 + 5) * (-0.2 * A34 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A34 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A34 + 5) * (-0.2 * A34 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A34 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>54.7</v>
       </c>
       <c r="C34" s="11">
-        <f>MIN(K$2, MAX(L$2, B34+N$2))</f>
+        <f>B34+O$2</f>
         <v>64.7</v>
       </c>
       <c r="D34" s="11">
-        <f>MIN(K$2, MAX(L$2, C34+O$2))</f>
+        <f t="shared" ref="D34:D65" si="2">C34+P$2</f>
         <v>68.7</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
-      <c r="N34" s="21"/>
-      <c r="O34" s="22"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E34" s="21">
+        <f t="shared" ref="E34:E65" si="3">MIN(L$2, MAX(M$2, D34))</f>
+        <v>68.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>-13</v>
       </c>
       <c r="B35" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A35 + 5) * (-0.2 * A35 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A35 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A35 + 5) * (-0.2 * A35 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A35 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>55.5</v>
       </c>
       <c r="C35" s="11">
-        <f>MIN(K$2, MAX(L$2, B35+N$2))</f>
+        <f>B35+O$2</f>
         <v>65.5</v>
       </c>
       <c r="D35" s="11">
-        <f>MIN(K$2, MAX(L$2, C35+O$2))</f>
+        <f t="shared" si="2"/>
         <v>69.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E35" s="21">
+        <f t="shared" si="3"/>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11">
         <v>-14</v>
       </c>
       <c r="B36" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A36 + 5) * (-0.2 * A36 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A36 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A36 + 5) * (-0.2 * A36 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A36 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>56.2</v>
       </c>
       <c r="C36" s="11">
-        <f>MIN(K$2, MAX(L$2, B36+N$2))</f>
+        <f>B36+O$2</f>
         <v>66.2</v>
       </c>
       <c r="D36" s="11">
-        <f>MIN(K$2, MAX(L$2, C36+O$2))</f>
+        <f t="shared" si="2"/>
         <v>70.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E36" s="21">
+        <f t="shared" si="3"/>
+        <v>70.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>-15</v>
       </c>
       <c r="B37" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A37 + 5) * (-0.2 * A37 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A37 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A37 + 5) * (-0.2 * A37 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A37 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>56.9</v>
       </c>
       <c r="C37" s="11">
-        <f>MIN(K$2, MAX(L$2, B37+N$2))</f>
+        <f>B37+O$2</f>
         <v>66.900000000000006</v>
       </c>
       <c r="D37" s="11">
-        <f>MIN(K$2, MAX(L$2, C37+O$2))</f>
+        <f t="shared" si="2"/>
         <v>70.900000000000006</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E37" s="21">
+        <f t="shared" si="3"/>
+        <v>70.900000000000006</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+      <c r="M37" s="13"/>
+      <c r="N37" s="13"/>
+      <c r="O37" s="13"/>
+      <c r="P37" s="14"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>-16</v>
       </c>
       <c r="B38" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A38 + 5) * (-0.2 * A38 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A38 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A38 + 5) * (-0.2 * A38 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A38 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>57.6</v>
       </c>
       <c r="C38" s="11">
-        <f>MIN(K$2, MAX(L$2, B38+N$2))</f>
+        <f>B38+O$2</f>
         <v>67.599999999999994</v>
       </c>
       <c r="D38" s="11">
-        <f>MIN(K$2, MAX(L$2, C38+O$2))</f>
+        <f t="shared" si="2"/>
         <v>71.599999999999994</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E38" s="21">
+        <f t="shared" si="3"/>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="17"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>-17</v>
       </c>
       <c r="B39" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A39 + 5) * (-0.2 * A39 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A39 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A39 + 5) * (-0.2 * A39 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A39 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>58.2</v>
       </c>
       <c r="C39" s="11">
-        <f>MIN(K$2, MAX(L$2, B39+N$2))</f>
+        <f>B39+O$2</f>
         <v>68.2</v>
       </c>
       <c r="D39" s="11">
-        <f>MIN(K$2, MAX(L$2, C39+O$2))</f>
+        <f t="shared" si="2"/>
         <v>72.2</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E39" s="21">
+        <f t="shared" si="3"/>
+        <v>72.2</v>
+      </c>
+      <c r="G39" s="15"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="17"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>-18</v>
       </c>
       <c r="B40" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A40 + 5) * (-0.2 * A40 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A40 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A40 + 5) * (-0.2 * A40 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A40 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>58.9</v>
       </c>
       <c r="C40" s="11">
-        <f>MIN(K$2, MAX(L$2, B40+N$2))</f>
+        <f>B40+O$2</f>
         <v>68.900000000000006</v>
       </c>
       <c r="D40" s="11">
-        <f>MIN(K$2, MAX(L$2, C40+O$2))</f>
+        <f t="shared" si="2"/>
         <v>72.900000000000006</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E40" s="21">
+        <f t="shared" si="3"/>
+        <v>72.900000000000006</v>
+      </c>
+      <c r="G40" s="15"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="17"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>-19</v>
       </c>
       <c r="B41" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A41 + 5) * (-0.2 * A41 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A41 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A41 + 5) * (-0.2 * A41 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A41 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>59.5</v>
       </c>
       <c r="C41" s="11">
-        <f>MIN(K$2, MAX(L$2, B41+N$2))</f>
+        <f>B41+O$2</f>
         <v>69.5</v>
       </c>
       <c r="D41" s="11">
-        <f>MIN(K$2, MAX(L$2, C41+O$2))</f>
+        <f t="shared" si="2"/>
         <v>73.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E41" s="21">
+        <f t="shared" si="3"/>
+        <v>73.5</v>
+      </c>
+      <c r="G41" s="15"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="17"/>
+    </row>
+    <row r="42" spans="1:16" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11">
         <v>-20</v>
       </c>
       <c r="B42" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A42 + 5) * (-0.2 * A42 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A42 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A42 + 5) * (-0.2 * A42 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A42 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>60.1</v>
       </c>
       <c r="C42" s="11">
-        <f>MIN(K$2, MAX(L$2, B42+N$2))</f>
+        <f>B42+O$2</f>
         <v>70.099999999999994</v>
       </c>
       <c r="D42" s="11">
-        <f>MIN(K$2, MAX(L$2, C42+O$2))</f>
+        <f t="shared" si="2"/>
         <v>74.099999999999994</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E42" s="21">
+        <f t="shared" si="3"/>
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G42" s="18"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="20"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>-21</v>
       </c>
       <c r="B43" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A43 + 5) * (-0.2 * A43 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A43 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A43 + 5) * (-0.2 * A43 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A43 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>60.7</v>
       </c>
       <c r="C43" s="11">
-        <f>MIN(K$2, MAX(L$2, B43+N$2))</f>
+        <f>B43+O$2</f>
         <v>70.7</v>
       </c>
       <c r="D43" s="11">
-        <f>MIN(K$2, MAX(L$2, C43+O$2))</f>
+        <f t="shared" si="2"/>
         <v>74.7</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E43" s="21">
+        <f t="shared" si="3"/>
+        <v>74.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>-22</v>
       </c>
       <c r="B44" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A44 + 5) * (-0.2 * A44 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A44 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A44 + 5) * (-0.2 * A44 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A44 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>61.2</v>
       </c>
       <c r="C44" s="11">
-        <f>MIN(K$2, MAX(L$2, B44+N$2))</f>
+        <f>B44+O$2</f>
         <v>71.2</v>
       </c>
       <c r="D44" s="11">
-        <f>MIN(K$2, MAX(L$2, C44+O$2))</f>
+        <f t="shared" si="2"/>
         <v>75.2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E44" s="21">
+        <f t="shared" si="3"/>
+        <v>75.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <v>-23</v>
       </c>
       <c r="B45" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A45 + 5) * (-0.2 * A45 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A45 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A45 + 5) * (-0.2 * A45 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A45 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>61.8</v>
       </c>
       <c r="C45" s="11">
-        <f>MIN(K$2, MAX(L$2, B45+N$2))</f>
+        <f>B45+O$2</f>
         <v>71.8</v>
       </c>
       <c r="D45" s="11">
-        <f>MIN(K$2, MAX(L$2, C45+O$2))</f>
+        <f t="shared" si="2"/>
         <v>75.8</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E45" s="21">
+        <f t="shared" si="3"/>
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>-24</v>
       </c>
       <c r="B46" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A46 + 5) * (-0.2 * A46 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A46 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A46 + 5) * (-0.2 * A46 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A46 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>62.3</v>
       </c>
       <c r="C46" s="11">
-        <f>MIN(K$2, MAX(L$2, B46+N$2))</f>
+        <f>B46+O$2</f>
         <v>72.3</v>
       </c>
       <c r="D46" s="11">
-        <f>MIN(K$2, MAX(L$2, C46+O$2))</f>
+        <f t="shared" si="2"/>
         <v>76.3</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E46" s="21">
+        <f t="shared" si="3"/>
+        <v>76.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>-25</v>
       </c>
       <c r="B47" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A47 + 5) * (-0.2 * A47 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A47 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A47 + 5) * (-0.2 * A47 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A47 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>62.8</v>
       </c>
       <c r="C47" s="11">
-        <f>MIN(K$2, MAX(L$2, B47+N$2))</f>
+        <f>B47+O$2</f>
         <v>72.8</v>
       </c>
       <c r="D47" s="11">
-        <f>MIN(K$2, MAX(L$2, C47+O$2))</f>
+        <f t="shared" si="2"/>
         <v>76.8</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="E47" s="21">
+        <f t="shared" si="3"/>
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>-26</v>
       </c>
       <c r="B48" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A48 + 5) * (-0.2 * A48 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A48 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A48 + 5) * (-0.2 * A48 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A48 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>63.2</v>
       </c>
       <c r="C48" s="11">
-        <f>MIN(K$2, MAX(L$2, B48+N$2))</f>
+        <f>B48+O$2</f>
         <v>73.2</v>
       </c>
       <c r="D48" s="11">
-        <f>MIN(K$2, MAX(L$2, C48+O$2))</f>
+        <f t="shared" si="2"/>
         <v>77.2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E48" s="21">
+        <f t="shared" si="3"/>
+        <v>77.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>-27</v>
       </c>
       <c r="B49" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A49 + 5) * (-0.2 * A49 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A49 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A49 + 5) * (-0.2 * A49 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A49 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>63.7</v>
       </c>
       <c r="C49" s="11">
-        <f>MIN(K$2, MAX(L$2, B49+N$2))</f>
+        <f>B49+O$2</f>
         <v>73.7</v>
       </c>
       <c r="D49" s="11">
-        <f>MIN(K$2, MAX(L$2, C49+O$2))</f>
+        <f t="shared" si="2"/>
         <v>77.7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E49" s="21">
+        <f t="shared" si="3"/>
+        <v>77.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>-28</v>
       </c>
       <c r="B50" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A50 + 5) * (-0.2 * A50 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A50 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A50 + 5) * (-0.2 * A50 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A50 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>64.099999999999994</v>
       </c>
       <c r="C50" s="11">
-        <f>MIN(K$2, MAX(L$2, B50+N$2))</f>
+        <f>B50+O$2</f>
         <v>74.099999999999994</v>
       </c>
       <c r="D50" s="11">
-        <f>MIN(K$2, MAX(L$2, C50+O$2))</f>
+        <f t="shared" si="2"/>
         <v>78.099999999999994</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E50" s="21">
+        <f t="shared" si="3"/>
+        <v>78.099999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>-29</v>
       </c>
       <c r="B51" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A51 + 5) * (-0.2 * A51 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A51 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A51 + 5) * (-0.2 * A51 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A51 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>64.599999999999994</v>
       </c>
       <c r="C51" s="11">
-        <f>MIN(K$2, MAX(L$2, B51+N$2))</f>
+        <f>B51+O$2</f>
         <v>74.599999999999994</v>
       </c>
       <c r="D51" s="11">
-        <f>MIN(K$2, MAX(L$2, C51+O$2))</f>
+        <f t="shared" si="2"/>
         <v>78.599999999999994</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E51" s="21">
+        <f t="shared" si="3"/>
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>-30</v>
       </c>
       <c r="B52" s="11">
-        <f>MIN(K$2, MAX(L$2, ROUND(((-0.21 * F$2 - 0.06) * (-0.2 * A52 + 5) * (-0.2 * A52 + 5)) + ((6.04 * F$2 + 1.98) * (-0.2 * A52 + 5)) + (-5.06 * F$2 + 18.06), 1)))</f>
+        <f>ROUND(((-0.21 * G$2 - 0.06) * (-0.2 * A52 + 5) * (-0.2 * A52 + 5)) + ((6.04 * G$2 + 1.98) * (-0.2 * A52 + 5)) + (-5.06 * G$2 + 18.06), 1)</f>
         <v>65</v>
       </c>
       <c r="C52" s="11">
-        <f>MIN(K$2, MAX(L$2, B52+N$2))</f>
+        <f>B52+O$2</f>
         <v>75</v>
       </c>
       <c r="D52" s="11">
-        <f>MIN(K$2, MAX(L$2, C52+O$2))</f>
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="E52" s="21">
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F29:O34"/>
+    <mergeCell ref="G37:P42"/>
   </mergeCells>
+  <conditionalFormatting sqref="A2:A52">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color theme="4"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color theme="4"/>
+        <color theme="2"/>
+        <color rgb="FFFF5050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>